<commit_message>
Added support for scraping electra race results website Updated league results
</commit_message>
<xml_diff>
--- a/RaceWebScraper/data/LigaOCRA/2 - MedievalXtremeRace-Polop-2024.xlsx
+++ b/RaceWebScraper/data/LigaOCRA/2 - MedievalXtremeRace-Polop-2024.xlsx
@@ -1690,7 +1690,7 @@
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="F39" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -1760,7 +1760,7 @@
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -1795,7 +1795,7 @@
       </c>
       <c r="F41" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G41" t="n">
@@ -1830,7 +1830,7 @@
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G42" t="n">
@@ -1865,7 +1865,7 @@
       </c>
       <c r="F43" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -1900,7 +1900,7 @@
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -1935,7 +1935,7 @@
       </c>
       <c r="F45" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G46" t="n">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -2300,7 +2300,7 @@
       </c>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -2335,7 +2335,7 @@
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -2370,7 +2370,7 @@
       </c>
       <c r="F11" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -2405,7 +2405,7 @@
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -3296,7 +3296,7 @@
       </c>
       <c r="F25" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -3331,7 +3331,7 @@
       </c>
       <c r="F26" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -3366,7 +3366,7 @@
       </c>
       <c r="F27" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="F28" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -3436,7 +3436,7 @@
       </c>
       <c r="F29" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -3471,7 +3471,7 @@
       </c>
       <c r="F30" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -3506,7 +3506,7 @@
       </c>
       <c r="F31" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -3541,7 +3541,7 @@
       </c>
       <c r="F32" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G32" t="n">
@@ -3576,7 +3576,7 @@
       </c>
       <c r="F33" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -3611,7 +3611,7 @@
       </c>
       <c r="F34" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -3646,7 +3646,7 @@
       </c>
       <c r="F35" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -3681,7 +3681,7 @@
       </c>
       <c r="F36" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -3716,7 +3716,7 @@
       </c>
       <c r="F37" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -3751,7 +3751,7 @@
       </c>
       <c r="F38" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -3786,7 +3786,7 @@
       </c>
       <c r="F39" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -3821,7 +3821,7 @@
       </c>
       <c r="F40" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -3856,7 +3856,7 @@
       </c>
       <c r="F41" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G41" t="n">
@@ -3891,7 +3891,7 @@
       </c>
       <c r="F42" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G42" t="n">
@@ -3926,7 +3926,7 @@
       </c>
       <c r="F43" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="F44" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -3996,7 +3996,7 @@
       </c>
       <c r="F45" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -4031,7 +4031,7 @@
       </c>
       <c r="F46" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G46" t="n">
@@ -4066,7 +4066,7 @@
       </c>
       <c r="F47" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G47" t="n">
@@ -4101,7 +4101,7 @@
       </c>
       <c r="F48" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -4136,7 +4136,7 @@
       </c>
       <c r="F49" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G49" t="n">
@@ -4171,7 +4171,7 @@
       </c>
       <c r="F50" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G50" t="n">
@@ -4206,7 +4206,7 @@
       </c>
       <c r="F51" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G51" t="n">
@@ -4241,7 +4241,7 @@
       </c>
       <c r="F52" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G52" t="n">
@@ -4276,7 +4276,7 @@
       </c>
       <c r="F53" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G53" t="n">
@@ -4311,7 +4311,7 @@
       </c>
       <c r="F54" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G54" t="n">
@@ -4346,7 +4346,7 @@
       </c>
       <c r="F55" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G55" t="n">
@@ -4381,7 +4381,7 @@
       </c>
       <c r="F56" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G56" t="n">
@@ -4416,7 +4416,7 @@
       </c>
       <c r="F57" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G57" t="n">
@@ -4451,7 +4451,7 @@
       </c>
       <c r="F58" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G58" t="n">
@@ -4486,7 +4486,7 @@
       </c>
       <c r="F59" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G59" t="n">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="F60" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G60" t="n">
@@ -4556,7 +4556,7 @@
       </c>
       <c r="F61" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G61" t="n">
@@ -4591,7 +4591,7 @@
       </c>
       <c r="F62" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G62" t="n">
@@ -4626,7 +4626,7 @@
       </c>
       <c r="F63" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G63" t="n">
@@ -4661,7 +4661,7 @@
       </c>
       <c r="F64" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G64" t="n">
@@ -4696,7 +4696,7 @@
       </c>
       <c r="F65" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G65" t="n">
@@ -4731,7 +4731,7 @@
       </c>
       <c r="F66" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G66" t="n">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="F67" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G67" t="n">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="F68" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G68" t="n">
@@ -4836,7 +4836,7 @@
       </c>
       <c r="F69" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G69" t="n">
@@ -4871,7 +4871,7 @@
       </c>
       <c r="F70" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G70" t="n">
@@ -4906,7 +4906,7 @@
       </c>
       <c r="F71" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G71" t="n">
@@ -4941,7 +4941,7 @@
       </c>
       <c r="F72" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G72" t="n">
@@ -4976,7 +4976,7 @@
       </c>
       <c r="F73" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G73" t="n">
@@ -5011,7 +5011,7 @@
       </c>
       <c r="F74" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G74" t="n">
@@ -5046,7 +5046,7 @@
       </c>
       <c r="F75" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G75" t="n">
@@ -5081,7 +5081,7 @@
       </c>
       <c r="F76" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G76" t="n">
@@ -5116,7 +5116,7 @@
       </c>
       <c r="F77" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G77" t="n">
@@ -5151,7 +5151,7 @@
       </c>
       <c r="F78" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G78" t="n">
@@ -5248,7 +5248,7 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -5283,7 +5283,7 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -5318,7 +5318,7 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -5353,7 +5353,7 @@
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -5388,7 +5388,7 @@
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -5423,7 +5423,7 @@
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -5458,7 +5458,7 @@
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -5493,7 +5493,7 @@
       </c>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -5528,7 +5528,7 @@
       </c>
       <c r="F10" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -5563,7 +5563,7 @@
       </c>
       <c r="F11" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -5598,7 +5598,7 @@
       </c>
       <c r="F12" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="F13" s="2" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>Descalificado</t>
         </is>
       </c>
       <c r="G13" t="n">

</xml_diff>